<commit_message>
Continue to add objects from libcntpr to Mile.NtCrt.Uefi.
</commit_message>
<xml_diff>
--- a/Mile.NtCrt.References/Lists/UefiCrtSymbolsList.xlsx
+++ b/Mile.NtCrt.References/Lists/UefiCrtSymbolsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ProjectMile\Mile.Windows.NtCrt\Mile.NtCrt.References\Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34180DD-46BA-46EB-90A0-E3E15B163C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63430D4E-6A34-4B73-A15D-1E854C9594AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="1296" windowWidth="34560" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="1416" windowWidth="34560" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UEFI CRT Symbols List" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="1071">
   <si>
     <t>arm64 Common Symbols</t>
   </si>
@@ -3237,6 +3237,10 @@
   </si>
   <si>
     <t>_fpieee_flt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_memicmp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3564,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C660"/>
+  <dimension ref="A1:C622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="A380" sqref="A380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6160,2784 +6164,2339 @@
         <v>438</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B308" s="1" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="B309" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>442</v>
+        <v>897</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>896</v>
+        <v>447</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B314" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>897</v>
+        <v>448</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>447</v>
+        <v>899</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="B319" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B320" s="1" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="B322" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="B324" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="B325" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="B326" s="1" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B327" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B328" s="1" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="B329" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="B330" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="B331" s="1" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>463</v>
+        <v>905</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>904</v>
+        <v>468</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>466</v>
+        <v>906</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>905</v>
+        <v>471</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>469</v>
+        <v>907</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>906</v>
+        <v>474</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>471</v>
+        <v>908</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>907</v>
+        <v>477</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>908</v>
+        <v>479</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>477</v>
+        <v>909</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>480</v>
+        <v>910</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>909</v>
+        <v>485</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>482</v>
+        <v>911</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>912</v>
+        <v>492</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>489</v>
+        <v>914</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>913</v>
+        <v>494</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>491</v>
+        <v>504</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>491</v>
+        <v>919</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>492</v>
+        <v>505</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>492</v>
+        <v>505</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>493</v>
+        <v>506</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>914</v>
+        <v>506</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>494</v>
+        <v>507</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>494</v>
+        <v>507</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>495</v>
+        <v>519</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>915</v>
+        <v>924</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>496</v>
+        <v>520</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>496</v>
+        <v>520</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>497</v>
+        <v>521</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>916</v>
+        <v>925</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>498</v>
+        <v>522</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>498</v>
+        <v>522</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>499</v>
+        <v>523</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>917</v>
+        <v>523</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>500</v>
+        <v>538</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>500</v>
+        <v>933</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>501</v>
+        <v>539</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>918</v>
+        <v>539</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>502</v>
+        <v>540</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>502</v>
+        <v>934</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>503</v>
+        <v>541</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>503</v>
+        <v>541</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>504</v>
+        <v>542</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>919</v>
+        <v>935</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>505</v>
+        <v>543</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>505</v>
+        <v>543</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>506</v>
+        <v>544</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>506</v>
+        <v>936</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>507</v>
+        <v>545</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>507</v>
+        <v>545</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>508</v>
+        <v>546</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>920</v>
+        <v>937</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>509</v>
+        <v>547</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>509</v>
+        <v>547</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>510</v>
+        <v>548</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>510</v>
+        <v>938</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>511</v>
+        <v>549</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>921</v>
+        <v>549</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>512</v>
+        <v>550</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>512</v>
+        <v>939</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>517</v>
+        <v>551</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>518</v>
+        <v>552</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>518</v>
+        <v>940</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>513</v>
+        <v>553</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>922</v>
+        <v>553</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>514</v>
+        <v>554</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>514</v>
+        <v>554</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>515</v>
+        <v>555</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>516</v>
+        <v>556</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>516</v>
+        <v>556</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>519</v>
+        <v>557</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>924</v>
+        <v>942</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>520</v>
+        <v>558</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>520</v>
+        <v>558</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>521</v>
+        <v>559</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>522</v>
+        <v>560</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>522</v>
+        <v>560</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>523</v>
+        <v>561</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>523</v>
+        <v>944</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>524</v>
+        <v>562</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>927</v>
+        <v>562</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>525</v>
+        <v>563</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>525</v>
+        <v>563</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>526</v>
+        <v>564</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>928</v>
+        <v>564</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>527</v>
+        <v>565</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>527</v>
+        <v>946</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>528</v>
+        <v>566</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>929</v>
+        <v>566</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="1" t="s">
-        <v>529</v>
-      </c>
       <c r="B398" s="1" t="s">
-        <v>529</v>
+        <v>945</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>530</v>
+        <v>567</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>930</v>
+        <v>567</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>531</v>
+        <v>568</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>531</v>
+        <v>947</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>532</v>
+        <v>569</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>931</v>
+        <v>569</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>533</v>
+        <v>570</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>533</v>
+        <v>948</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>534</v>
+        <v>571</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>926</v>
+        <v>571</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>535</v>
+        <v>572</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>535</v>
+        <v>949</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>536</v>
+        <v>573</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>932</v>
+        <v>573</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>537</v>
+        <v>574</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>537</v>
+        <v>950</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>538</v>
+        <v>575</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>933</v>
+        <v>575</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>539</v>
+        <v>576</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>539</v>
+        <v>951</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>540</v>
+        <v>577</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>934</v>
+        <v>577</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>541</v>
+        <v>578</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>541</v>
+        <v>952</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
-        <v>542</v>
+        <v>579</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>935</v>
+        <v>579</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>543</v>
+        <v>580</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>543</v>
+        <v>953</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>544</v>
+        <v>581</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>936</v>
+        <v>581</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>545</v>
+        <v>582</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>545</v>
+        <v>954</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>546</v>
+        <v>583</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>937</v>
+        <v>583</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>547</v>
+        <v>584</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>547</v>
+        <v>955</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>548</v>
+        <v>585</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>938</v>
+        <v>585</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>549</v>
+        <v>586</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>549</v>
+        <v>956</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>550</v>
+        <v>587</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>939</v>
+        <v>587</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>551</v>
+        <v>588</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>551</v>
+        <v>957</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>552</v>
+        <v>589</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>940</v>
+        <v>589</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>553</v>
+        <v>590</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>553</v>
+        <v>958</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>554</v>
+        <v>591</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>554</v>
+        <v>591</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>941</v>
+        <v>959</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>556</v>
+        <v>593</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>556</v>
+        <v>593</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>557</v>
+        <v>594</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>942</v>
+        <v>960</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>558</v>
+        <v>595</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>558</v>
+        <v>595</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>559</v>
+        <v>596</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>943</v>
+        <v>961</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>560</v>
+        <v>597</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>560</v>
+        <v>597</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>561</v>
+        <v>598</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>944</v>
+        <v>962</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>562</v>
+        <v>599</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>562</v>
+        <v>599</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>563</v>
+        <v>600</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>563</v>
+        <v>963</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>564</v>
+        <v>601</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>564</v>
+        <v>601</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
-        <v>565</v>
+        <v>602</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>946</v>
+        <v>964</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
-        <v>566</v>
+        <v>603</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>566</v>
+        <v>603</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="1" t="s">
+        <v>665</v>
+      </c>
       <c r="B436" s="1" t="s">
-        <v>945</v>
+        <v>997</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>567</v>
+        <v>666</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>567</v>
+        <v>666</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="1" t="s">
-        <v>568</v>
-      </c>
       <c r="B438" s="1" t="s">
-        <v>947</v>
+        <v>965</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
-        <v>569</v>
+        <v>667</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>569</v>
+        <v>667</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
-        <v>570</v>
+        <v>604</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>948</v>
+        <v>966</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
-        <v>571</v>
+        <v>605</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>571</v>
+        <v>605</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>572</v>
+        <v>606</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>949</v>
+        <v>967</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>573</v>
+        <v>607</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>573</v>
+        <v>607</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
-        <v>574</v>
+        <v>608</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>950</v>
+        <v>968</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>576</v>
+        <v>610</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>951</v>
+        <v>969</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
-        <v>577</v>
+        <v>611</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>577</v>
+        <v>611</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>952</v>
+        <v>970</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
-        <v>579</v>
+        <v>613</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>579</v>
+        <v>613</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
-        <v>580</v>
+        <v>614</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>953</v>
+        <v>971</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
-        <v>581</v>
+        <v>615</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>581</v>
+        <v>615</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>954</v>
+        <v>975</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
-        <v>583</v>
+        <v>617</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>583</v>
+        <v>617</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
-        <v>584</v>
+        <v>618</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>955</v>
+        <v>976</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
-        <v>585</v>
+        <v>619</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>585</v>
+        <v>619</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>956</v>
+        <v>977</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
-        <v>587</v>
+        <v>621</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>587</v>
+        <v>621</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
-        <v>588</v>
+        <v>622</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>957</v>
+        <v>979</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
-        <v>589</v>
+        <v>623</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>589</v>
+        <v>623</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
-        <v>590</v>
+        <v>624</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>958</v>
+        <v>980</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
-        <v>591</v>
+        <v>625</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>591</v>
+        <v>625</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
-        <v>592</v>
+        <v>626</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>959</v>
+        <v>981</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
-        <v>593</v>
+        <v>627</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>593</v>
+        <v>627</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
-        <v>594</v>
+        <v>628</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>960</v>
+        <v>628</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
-        <v>595</v>
+        <v>629</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>595</v>
+        <v>982</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
-        <v>596</v>
+        <v>630</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>961</v>
+        <v>630</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
-        <v>597</v>
+        <v>631</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>597</v>
+        <v>983</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
-        <v>598</v>
+        <v>632</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>962</v>
+        <v>632</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" s="1" t="s">
-        <v>599</v>
+        <v>633</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>599</v>
+        <v>984</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
-        <v>600</v>
+        <v>1068</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>963</v>
+        <v>634</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" s="1" t="s">
-        <v>601</v>
+        <v>635</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>601</v>
+        <v>985</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
-        <v>602</v>
+        <v>636</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>964</v>
+        <v>636</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
-        <v>603</v>
+        <v>637</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>603</v>
+        <v>986</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
-        <v>665</v>
+        <v>638</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>997</v>
+        <v>638</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" s="1" t="s">
-        <v>666</v>
+        <v>639</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>666</v>
+        <v>987</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" s="1" t="s">
+        <v>640</v>
+      </c>
       <c r="B476" s="1" t="s">
-        <v>965</v>
+        <v>640</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" s="1" t="s">
-        <v>667</v>
+        <v>641</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>667</v>
+        <v>988</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
-        <v>604</v>
+        <v>642</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>966</v>
+        <v>642</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
-        <v>605</v>
+        <v>643</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>605</v>
+        <v>989</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
-        <v>606</v>
+        <v>644</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>967</v>
+        <v>644</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" s="1" t="s">
-        <v>607</v>
+        <v>645</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>607</v>
+        <v>990</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" s="1" t="s">
-        <v>608</v>
+        <v>646</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>968</v>
+        <v>646</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" s="1" t="s">
-        <v>609</v>
+        <v>647</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>609</v>
+        <v>647</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
-        <v>610</v>
+        <v>648</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>969</v>
+        <v>648</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" s="1" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
-        <v>612</v>
+        <v>650</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>970</v>
+        <v>650</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" s="1" t="s">
-        <v>613</v>
+        <v>651</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>613</v>
+        <v>651</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
-        <v>614</v>
+        <v>652</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>971</v>
+        <v>991</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" s="1" t="s">
-        <v>615</v>
+        <v>653</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>615</v>
+        <v>653</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
-        <v>616</v>
+        <v>654</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>975</v>
+        <v>992</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" s="1" t="s">
-        <v>617</v>
+        <v>655</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>617</v>
+        <v>655</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
-        <v>618</v>
+        <v>656</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
-        <v>619</v>
+        <v>657</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>619</v>
+        <v>657</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A494" s="1" t="s">
-        <v>620</v>
-      </c>
       <c r="B494" s="1" t="s">
-        <v>977</v>
+        <v>993</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" s="1" t="s">
-        <v>621</v>
+        <v>658</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>621</v>
+        <v>658</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
-        <v>622</v>
+        <v>659</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>979</v>
+        <v>994</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" s="1" t="s">
-        <v>623</v>
+        <v>660</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>623</v>
+        <v>660</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
-        <v>624</v>
+        <v>661</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>980</v>
+        <v>995</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" s="1" t="s">
-        <v>625</v>
+        <v>662</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>625</v>
+        <v>662</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
-        <v>626</v>
+        <v>663</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>981</v>
+        <v>996</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" s="1" t="s">
-        <v>627</v>
+        <v>664</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>627</v>
+        <v>664</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" s="1" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>628</v>
+        <v>998</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" s="1" t="s">
-        <v>629</v>
+        <v>669</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>982</v>
+        <v>669</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" s="1" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>630</v>
+        <v>973</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" s="1" t="s">
-        <v>631</v>
+        <v>671</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>983</v>
+        <v>671</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" s="1" t="s">
-        <v>632</v>
+        <v>674</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>632</v>
+        <v>974</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" s="1" t="s">
-        <v>633</v>
+        <v>675</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>984</v>
+        <v>675</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A508" s="1" t="s">
-        <v>1068</v>
-      </c>
       <c r="B508" s="1" t="s">
-        <v>634</v>
+        <v>999</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" s="1" t="s">
-        <v>635</v>
+        <v>676</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>985</v>
+        <v>676</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" s="1" t="s">
-        <v>636</v>
+        <v>677</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>636</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" s="1" t="s">
-        <v>637</v>
+        <v>678</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>986</v>
+        <v>678</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
-        <v>638</v>
+        <v>679</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>638</v>
+        <v>679</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" s="1" t="s">
-        <v>639</v>
+        <v>680</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>987</v>
+        <v>680</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
-        <v>640</v>
+        <v>681</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>640</v>
+        <v>681</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" s="1" t="s">
-        <v>641</v>
+        <v>682</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>988</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
-        <v>642</v>
+        <v>683</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>642</v>
+        <v>683</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" s="1" t="s">
-        <v>643</v>
+        <v>684</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>989</v>
+        <v>684</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" s="1" t="s">
-        <v>644</v>
+        <v>685</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>644</v>
+        <v>685</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" s="1" t="s">
-        <v>645</v>
+        <v>686</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>990</v>
+        <v>686</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" s="1" t="s">
-        <v>646</v>
+        <v>687</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>646</v>
+        <v>687</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" s="1" t="s">
-        <v>647</v>
+        <v>688</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>647</v>
+        <v>688</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
-        <v>648</v>
+        <v>689</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>648</v>
+        <v>689</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" s="1" t="s">
-        <v>649</v>
+        <v>690</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>649</v>
+        <v>690</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" s="1" t="s">
-        <v>650</v>
+        <v>691</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>650</v>
+        <v>691</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" s="1" t="s">
-        <v>651</v>
+        <v>692</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>651</v>
+        <v>692</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" s="1" t="s">
-        <v>652</v>
+        <v>693</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>991</v>
+        <v>693</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" s="1" t="s">
-        <v>653</v>
+        <v>694</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>653</v>
+        <v>694</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" s="1" t="s">
-        <v>654</v>
+        <v>695</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>992</v>
+        <v>695</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" s="1" t="s">
-        <v>655</v>
+        <v>696</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>655</v>
+        <v>696</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" s="1" t="s">
-        <v>656</v>
+        <v>697</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>972</v>
+        <v>697</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" s="1" t="s">
-        <v>657</v>
+        <v>698</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>657</v>
+        <v>698</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A532" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="B532" s="1" t="s">
-        <v>993</v>
+        <v>699</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" s="1" t="s">
-        <v>658</v>
+        <v>700</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>658</v>
+        <v>700</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" s="1" t="s">
-        <v>659</v>
+        <v>701</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>994</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" s="1" t="s">
-        <v>660</v>
+        <v>702</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>660</v>
+        <v>702</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" s="1" t="s">
-        <v>661</v>
+        <v>703</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" s="1" t="s">
-        <v>662</v>
+        <v>704</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="538" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A538" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="B538" s="1" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A539" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="B539" s="1" t="s">
-        <v>664</v>
+        <v>704</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" s="1" t="s">
-        <v>668</v>
+        <v>707</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>998</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" s="1" t="s">
-        <v>669</v>
+        <v>708</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>669</v>
+        <v>708</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" s="1" t="s">
-        <v>670</v>
+        <v>709</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>973</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" s="1" t="s">
-        <v>671</v>
+        <v>710</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>671</v>
+        <v>710</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" s="1" t="s">
-        <v>674</v>
+        <v>711</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>974</v>
+        <v>711</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" s="1" t="s">
-        <v>675</v>
+        <v>712</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>675</v>
+        <v>712</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A546" s="1" t="s">
+        <v>713</v>
+      </c>
       <c r="B546" s="1" t="s">
-        <v>999</v>
+        <v>713</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" s="1" t="s">
-        <v>676</v>
+        <v>714</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>676</v>
+        <v>714</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" s="1" t="s">
-        <v>677</v>
+        <v>715</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1000</v>
+        <v>715</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" s="1" t="s">
-        <v>678</v>
+        <v>716</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>678</v>
+        <v>978</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" s="1" t="s">
-        <v>679</v>
+        <v>717</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>679</v>
+        <v>717</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" s="1" t="s">
-        <v>680</v>
+        <v>718</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>680</v>
+        <v>718</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A552" s="1" t="s">
-        <v>681</v>
+        <v>719</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>681</v>
+        <v>719</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" s="1" t="s">
-        <v>682</v>
+        <v>720</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1001</v>
+        <v>720</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A554" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="B554" s="1" t="s">
-        <v>683</v>
+        <v>672</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>684</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" s="1" t="s">
-        <v>685</v>
+        <v>721</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>685</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" s="1" t="s">
-        <v>686</v>
+        <v>722</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>686</v>
+        <v>722</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" s="1" t="s">
-        <v>687</v>
+        <v>723</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>687</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" s="1" t="s">
-        <v>688</v>
+        <v>724</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>688</v>
+        <v>724</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" s="1" t="s">
-        <v>689</v>
+        <v>725</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>689</v>
+        <v>725</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A561" s="1" t="s">
-        <v>690</v>
+        <v>726</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>690</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" s="1" t="s">
-        <v>691</v>
+        <v>727</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>691</v>
+        <v>727</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" s="1" t="s">
-        <v>692</v>
+        <v>728</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>692</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" s="1" t="s">
-        <v>693</v>
+        <v>729</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>693</v>
+        <v>729</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" s="1" t="s">
-        <v>694</v>
+        <v>730</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>694</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" s="1" t="s">
-        <v>695</v>
+        <v>731</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>695</v>
+        <v>731</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" s="1" t="s">
-        <v>696</v>
+        <v>732</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>696</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" s="1" t="s">
-        <v>697</v>
+        <v>733</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>697</v>
+        <v>733</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" s="1" t="s">
-        <v>698</v>
+        <v>734</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>698</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" s="1" t="s">
-        <v>699</v>
+        <v>735</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>699</v>
+        <v>735</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" s="1" t="s">
-        <v>700</v>
+        <v>736</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>700</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" s="1" t="s">
-        <v>701</v>
+        <v>737</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1003</v>
+        <v>737</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" s="1" t="s">
-        <v>702</v>
+        <v>738</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>702</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" s="1" t="s">
-        <v>703</v>
+        <v>739</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1002</v>
+        <v>739</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" s="1" t="s">
-        <v>704</v>
+        <v>740</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>704</v>
+        <v>740</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A576" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" s="1" t="s">
-        <v>707</v>
+        <v>743</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1005</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" s="1" t="s">
-        <v>708</v>
+        <v>744</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>708</v>
+        <v>744</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" s="1" t="s">
-        <v>709</v>
+        <v>745</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1006</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" s="1" t="s">
-        <v>710</v>
+        <v>746</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>710</v>
+        <v>746</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" s="1" t="s">
-        <v>711</v>
+        <v>747</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>711</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" s="1" t="s">
-        <v>712</v>
+        <v>748</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>712</v>
+        <v>748</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" s="1" t="s">
-        <v>713</v>
+        <v>749</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>713</v>
+        <v>749</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" s="1" t="s">
-        <v>714</v>
+        <v>750</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>714</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" s="1" t="s">
-        <v>715</v>
+        <v>751</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>715</v>
+        <v>751</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" s="1" t="s">
-        <v>716</v>
+        <v>752</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>978</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" s="1" t="s">
-        <v>717</v>
+        <v>753</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>717</v>
+        <v>753</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" s="1" t="s">
-        <v>718</v>
+        <v>754</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>718</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" s="1" t="s">
-        <v>719</v>
+        <v>755</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>719</v>
+        <v>755</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" s="1" t="s">
-        <v>720</v>
+        <v>756</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>720</v>
+        <v>756</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" s="1" t="s">
-        <v>672</v>
+        <v>757</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" s="1" t="s">
-        <v>1069</v>
+        <v>758</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" s="1" t="s">
-        <v>721</v>
+        <v>759</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>1007</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" s="1" t="s">
-        <v>722</v>
+        <v>760</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>722</v>
+        <v>760</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" s="1" t="s">
-        <v>723</v>
+        <v>761</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>1008</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" s="1" t="s">
-        <v>724</v>
+        <v>762</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>724</v>
+        <v>762</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A598" s="1" t="s">
-        <v>725</v>
-      </c>
       <c r="B598" s="1" t="s">
-        <v>725</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A599" s="1" t="s">
-        <v>726</v>
-      </c>
       <c r="B599" s="1" t="s">
-        <v>1009</v>
+        <v>673</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" s="1" t="s">
-        <v>727</v>
+        <v>763</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>727</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" s="1" t="s">
-        <v>728</v>
+        <v>764</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>1010</v>
+        <v>764</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" s="1" t="s">
-        <v>729</v>
+        <v>765</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>729</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" s="1" t="s">
-        <v>730</v>
+        <v>766</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>1011</v>
+        <v>766</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" s="1" t="s">
-        <v>731</v>
+        <v>767</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>731</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" s="1" t="s">
-        <v>732</v>
+        <v>768</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>1012</v>
+        <v>768</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" s="1" t="s">
-        <v>733</v>
+        <v>769</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>733</v>
+        <v>769</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" s="1" t="s">
-        <v>734</v>
+        <v>770</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>1013</v>
+        <v>770</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" s="1" t="s">
-        <v>735</v>
+        <v>771</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>735</v>
+        <v>771</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" s="1" t="s">
-        <v>736</v>
+        <v>772</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>1014</v>
+        <v>772</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" s="1" t="s">
-        <v>737</v>
+        <v>773</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>737</v>
+        <v>773</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" s="1" t="s">
-        <v>738</v>
+        <v>774</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>1015</v>
+        <v>774</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" s="1" t="s">
-        <v>739</v>
+        <v>775</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>739</v>
+        <v>775</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" s="1" t="s">
-        <v>740</v>
+        <v>776</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>740</v>
+        <v>776</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" s="1" t="s">
-        <v>741</v>
+        <v>777</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>1016</v>
+        <v>777</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" s="1" t="s">
-        <v>742</v>
+        <v>778</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>742</v>
+        <v>778</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" s="1" t="s">
-        <v>743</v>
+        <v>1</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>1017</v>
+        <v>1</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" s="1" t="s">
-        <v>744</v>
+        <v>70</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>744</v>
+        <v>793</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" s="1" t="s">
-        <v>745</v>
+        <v>71</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>1018</v>
+        <v>71</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" s="1" t="s">
-        <v>746</v>
+        <v>72</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>746</v>
+        <v>72</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" s="1" t="s">
-        <v>747</v>
+        <v>92</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>1019</v>
+        <v>800</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" s="1" t="s">
-        <v>748</v>
+        <v>93</v>
       </c>
       <c r="B621" s="1" t="s">
-        <v>748</v>
+        <v>93</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" s="1" t="s">
-        <v>749</v>
+        <v>94</v>
       </c>
       <c r="B622" s="1" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A623" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="B623" s="1" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A624" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="B624" s="1" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A625" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="B625" s="1" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A626" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="B626" s="1" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A627" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="B627" s="1" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A628" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="B628" s="1" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A629" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="B629" s="1" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A630" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="B630" s="1" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A631" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="B631" s="1" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A632" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="B632" s="1" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A633" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="B633" s="1" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A634" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="B634" s="1" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A635" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="B635" s="1" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B636" s="1" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B637" s="1" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A638" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="B638" s="1" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A639" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="B639" s="1" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A640" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="B640" s="1" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A641" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="B641" s="1" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A642" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="B642" s="1" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A643" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="B643" s="1" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A644" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="B644" s="1" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A645" s="1" t="s">
-        <v>770</v>
-      </c>
-      <c r="B645" s="1" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A646" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="B646" s="1" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A647" s="1" t="s">
-        <v>772</v>
-      </c>
-      <c r="B647" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A648" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="B648" s="1" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A649" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="B649" s="1" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A650" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="B650" s="1" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A651" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="B651" s="1" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A652" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="B652" s="1" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A653" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="B653" s="1" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A654" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B654" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A655" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B655" s="1" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A656" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B656" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A657" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B657" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A658" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B658" s="1" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A659" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B659" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A660" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B660" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -8949,10 +8508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81ADE4D5-49C9-4B3A-AAC3-C72CBEBC9A41}">
-  <dimension ref="A1:B129"/>
+  <dimension ref="A1:B185"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B111" sqref="B110:B111"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -9994,6 +9553,452 @@
         <v>136</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>